<commit_message>
changing hours on plan
</commit_message>
<xml_diff>
--- a/LITZ_ProjectPlanner.xlsx
+++ b/LITZ_ProjectPlanner.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\GitHub\LITZombies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sinead\Documents\GitHub\LITZombies\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -614,7 +614,7 @@
   <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,7 +713,7 @@
         <v>6</v>
       </c>
       <c r="G6" s="13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="9" t="s">

</xml_diff>

<commit_message>
Anding the weeks that eash task should be done.
</commit_message>
<xml_diff>
--- a/LITZ_ProjectPlanner.xlsx
+++ b/LITZ_ProjectPlanner.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="72">
   <si>
     <t>Learning/Logging</t>
   </si>
@@ -213,6 +213,33 @@
   </si>
   <si>
     <t>one-liners (lecturers)</t>
+  </si>
+  <si>
+    <t>Weeks Assigned</t>
+  </si>
+  <si>
+    <t>Week 1-3</t>
+  </si>
+  <si>
+    <t>Week 2-3</t>
+  </si>
+  <si>
+    <t>Week 1-2</t>
+  </si>
+  <si>
+    <t>Week 2-4</t>
+  </si>
+  <si>
+    <t>Week 2-7</t>
+  </si>
+  <si>
+    <t>Week 3-9</t>
+  </si>
+  <si>
+    <t>Week 5-11</t>
+  </si>
+  <si>
+    <t>Week 12</t>
   </si>
 </sst>
 </file>
@@ -288,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -323,6 +350,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -611,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J65"/>
+  <dimension ref="A1:O65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="L63" sqref="L63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +653,7 @@
     <col min="8" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -634,8 +664,11 @@
       <c r="I1" s="7" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L1" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -652,8 +685,11 @@
       <c r="J2" s="10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L2" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -668,8 +704,11 @@
         <v>60</v>
       </c>
       <c r="J3" s="10"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -686,8 +725,11 @@
       <c r="J4" s="10" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -705,7 +747,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -723,14 +765,14 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="G7" s="13"/>
       <c r="H7" s="1"/>
       <c r="I7" s="9"/>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
@@ -739,7 +781,7 @@
       <c r="I8" s="9"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -756,8 +798,12 @@
       <c r="J9" s="10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>66</v>
+      </c>
+      <c r="O9" s="14"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -770,8 +816,11 @@
       <c r="J10" s="10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
@@ -784,8 +833,11 @@
         <v>60</v>
       </c>
       <c r="J11" s="10"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -800,15 +852,18 @@
       <c r="J12" s="10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="G13" s="13"/>
       <c r="H13" s="1"/>
       <c r="I13" s="9"/>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
@@ -817,7 +872,7 @@
       <c r="I14" s="9"/>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
@@ -830,8 +885,11 @@
       <c r="J15" s="10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
         <v>2</v>
@@ -846,7 +904,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2" t="s">
         <v>2</v>
@@ -861,7 +919,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2" t="s">
         <v>2</v>
@@ -876,7 +934,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2" t="s">
         <v>2</v>
@@ -891,7 +949,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2" t="s">
         <v>2</v>
@@ -906,7 +964,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2" t="s">
         <v>2</v>
@@ -921,7 +979,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>2</v>
       </c>
@@ -935,7 +993,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>2</v>
       </c>
@@ -949,13 +1007,13 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G24" s="13"/>
       <c r="H24" s="1"/>
       <c r="I24" s="9"/>
       <c r="J24" s="10"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>2</v>
       </c>
@@ -967,7 +1025,7 @@
       <c r="I25" s="9"/>
       <c r="J25" s="10"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>2</v>
       </c>
@@ -982,8 +1040,11 @@
       <c r="J26" s="10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>2</v>
       </c>
@@ -997,7 +1058,7 @@
       </c>
       <c r="J27" s="10"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
         <v>2</v>
       </c>
@@ -1011,7 +1072,7 @@
       </c>
       <c r="J28" s="10"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C29" s="2" t="s">
         <v>2</v>
       </c>
@@ -1025,7 +1086,7 @@
       </c>
       <c r="J29" s="10"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C30" s="2" t="s">
         <v>2</v>
       </c>
@@ -1039,7 +1100,7 @@
       </c>
       <c r="J30" s="10"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C31" s="2" t="s">
         <v>2</v>
       </c>
@@ -1053,7 +1114,7 @@
       </c>
       <c r="J31" s="10"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C32" s="2" t="s">
         <v>2</v>
       </c>
@@ -1067,7 +1128,7 @@
       </c>
       <c r="J32" s="10"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C33" s="2" t="s">
         <v>2</v>
       </c>
@@ -1081,7 +1142,7 @@
       </c>
       <c r="J33" s="10"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C34" s="2" t="s">
         <v>2</v>
       </c>
@@ -1095,7 +1156,7 @@
       </c>
       <c r="J34" s="10"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C35" s="2" t="s">
         <v>2</v>
       </c>
@@ -1109,13 +1170,13 @@
       </c>
       <c r="J35" s="10"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G36" s="13"/>
       <c r="H36" s="1"/>
       <c r="I36" s="9"/>
       <c r="J36" s="10"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>2</v>
       </c>
@@ -1126,8 +1187,11 @@
       <c r="H37" s="1"/>
       <c r="I37" s="9"/>
       <c r="J37" s="10"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>2</v>
       </c>
@@ -1141,7 +1205,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>2</v>
       </c>
@@ -1155,7 +1219,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>2</v>
       </c>
@@ -1167,7 +1231,7 @@
       <c r="I40" s="9"/>
       <c r="J40" s="10"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C41" s="2" t="s">
         <v>2</v>
       </c>
@@ -1181,7 +1245,7 @@
       </c>
       <c r="J41" s="10"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C42" s="2" t="s">
         <v>2</v>
       </c>
@@ -1195,7 +1259,7 @@
       </c>
       <c r="J42" s="10"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C43" s="2" t="s">
         <v>2</v>
       </c>
@@ -1209,7 +1273,7 @@
       </c>
       <c r="J43" s="10"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C44" s="2" t="s">
         <v>2</v>
       </c>
@@ -1223,7 +1287,7 @@
       </c>
       <c r="J44" s="10"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
         <v>2</v>
       </c>
@@ -1235,7 +1299,7 @@
       <c r="I45" s="9"/>
       <c r="J45" s="10"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C46" s="2" t="s">
         <v>2</v>
       </c>
@@ -1249,7 +1313,7 @@
       </c>
       <c r="J46" s="10"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C47" s="2" t="s">
         <v>2</v>
       </c>
@@ -1263,7 +1327,7 @@
       </c>
       <c r="J47" s="10"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C48" s="2" t="s">
         <v>2</v>
       </c>
@@ -1277,7 +1341,7 @@
       </c>
       <c r="J48" s="10"/>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C49" s="2" t="s">
         <v>2</v>
       </c>
@@ -1291,7 +1355,7 @@
       </c>
       <c r="J49" s="10"/>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C50" s="2" t="s">
         <v>2</v>
       </c>
@@ -1305,7 +1369,7 @@
       </c>
       <c r="J50" s="10"/>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
         <v>2</v>
       </c>
@@ -1317,7 +1381,7 @@
       <c r="I51" s="9"/>
       <c r="J51" s="10"/>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C52" s="2" t="s">
         <v>2</v>
       </c>
@@ -1331,7 +1395,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C53" s="2" t="s">
         <v>2</v>
       </c>
@@ -1345,7 +1409,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C54" s="2" t="s">
         <v>2</v>
       </c>
@@ -1359,7 +1423,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
         <v>2</v>
       </c>
@@ -1371,7 +1435,7 @@
       <c r="I55" s="9"/>
       <c r="J55" s="10"/>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
         <v>2</v>
       </c>
@@ -1385,7 +1449,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>2</v>
       </c>
@@ -1399,7 +1463,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C58" s="2" t="s">
         <v>2</v>
       </c>
@@ -1413,7 +1477,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
         <v>2</v>
       </c>
@@ -1427,7 +1491,7 @@
       </c>
       <c r="J59" s="10"/>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
         <v>2</v>
       </c>
@@ -1439,7 +1503,7 @@
       <c r="I60" s="9"/>
       <c r="J60" s="10"/>
     </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C61" s="2" t="s">
         <v>2</v>
       </c>
@@ -1453,7 +1517,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C62" s="2" t="s">
         <v>2</v>
       </c>
@@ -1467,7 +1531,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
         <v>2</v>
       </c>
@@ -1481,6 +1545,9 @@
       </c>
       <c r="J63" s="10" t="s">
         <v>61</v>
+      </c>
+      <c r="L63" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="65" spans="9:10" x14ac:dyDescent="0.25">

</xml_diff>